<commit_message>
Site updated: 2020-05-20 22:03:23
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094F7199-5222-4596-A222-C5457C4F9FE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD39DC-CA6A-4EF1-A48E-25185C44EE21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,6 +279,12 @@
   <si>
     <t>datawhale</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>Recommendation System</t>
   </si>
 </sst>
 </file>
@@ -645,7 +651,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -745,6 +751,9 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
@@ -827,6 +836,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
       <c r="H8" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Site updated: 2020-05-27 14:24:31
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD39DC-CA6A-4EF1-A48E-25185C44EE21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89672B2D-E905-4852-B5BF-F83C7C846724}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>Recommendation System</t>
+  </si>
+  <si>
+    <t>Data Augmentation</t>
+  </si>
+  <si>
+    <t>Digit Recognition</t>
   </si>
 </sst>
 </file>
@@ -651,7 +657,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -825,6 +831,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
@@ -836,6 +845,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
       <c r="C8" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Site updated: 2020-05-30 22:18:10
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89672B2D-E905-4852-B5BF-F83C7C846724}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3C6A4-557B-4336-A360-8D4F26EDE09D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -291,6 +291,13 @@
   </si>
   <si>
     <t>Digit Recognition</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Verification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -657,7 +664,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -786,6 +793,9 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
       <c r="G4" t="s">
         <v>33</v>
       </c>
@@ -805,6 +815,9 @@
       </c>
       <c r="C5" t="s">
         <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Site updated: 2020-06-02 14:26:03
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3C6A4-557B-4336-A360-8D4F26EDE09D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B244F7E3-9C12-488B-A6EF-BCAB767D8C5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,6 +298,34 @@
   <si>
     <t>Verification</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slice</t>
+  </si>
+  <si>
+    <t>移动硬盘</t>
+  </si>
+  <si>
+    <t>concatenate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fuzz Testing</t>
+  </si>
+  <si>
+    <t>Robustness</t>
+  </si>
+  <si>
+    <t>Deep Neural Networks</t>
+  </si>
+  <si>
+    <t>Adversarial Attacks</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>Text Classification</t>
   </si>
 </sst>
 </file>
@@ -661,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF1DB48-2DFC-4ED4-8546-E0DC9CD3BD21}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -782,6 +810,9 @@
       <c r="K3" t="s">
         <v>26</v>
       </c>
+      <c r="L3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
@@ -811,7 +842,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -831,11 +862,14 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
@@ -845,11 +879,14 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
+      <c r="F7" t="s">
+        <v>85</v>
+      </c>
       <c r="H7" t="s">
         <v>30</v>
       </c>
@@ -859,21 +896,33 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>76</v>
       </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" t="s">
         <v>31</v>
       </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
       <c r="H9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
       <c r="H10" t="s">
         <v>35</v>
       </c>
@@ -906,6 +955,16 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="H16" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.4">
+      <c r="H17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.4">
+      <c r="H18" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2020-06-03 22:42:35
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B244F7E3-9C12-488B-A6EF-BCAB767D8C5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F618836C-5C1A-4AD3-B111-3B47AF615481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -326,6 +326,23 @@
   </si>
   <si>
     <t>Text Classification</t>
+  </si>
+  <si>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t>Bagging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SaveModel</t>
+  </si>
+  <si>
+    <t>TensorFlow</t>
   </si>
 </sst>
 </file>
@@ -692,7 +709,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -912,6 +929,12 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
       <c r="F9" t="s">
         <v>37</v>
       </c>
@@ -920,6 +943,12 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
       <c r="F10" t="s">
         <v>87</v>
       </c>
@@ -928,6 +957,9 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
       <c r="H11" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Site updated: 2020-06-08 10:15:27
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F618836C-5C1A-4AD3-B111-3B47AF615481}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7326A7D-D64F-4581-BF1B-AB8E01628A82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,6 +343,14 @@
   </si>
   <si>
     <t>TensorFlow</t>
+  </si>
+  <si>
+    <t>Windows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PowerOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -709,7 +717,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -864,6 +872,9 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
       <c r="F5" t="s">
         <v>80</v>
       </c>
@@ -883,6 +894,9 @@
       </c>
       <c r="C6" t="s">
         <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
       </c>
       <c r="F6" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Site updated: 2020-06-23 21:14:06
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7326A7D-D64F-4581-BF1B-AB8E01628A82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7EFD9-62D0-461C-8004-10FF4B3B265B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -350,6 +350,10 @@
   </si>
   <si>
     <t>PowerOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keras</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -717,7 +721,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -979,6 +983,9 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
       <c r="H12" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Site updated: 2020-07-20 17:00:58
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF7EFD9-62D0-461C-8004-10FF4B3B265B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CDBB76-7884-4064-A281-79A19471F979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>RNN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -355,6 +355,12 @@
   <si>
     <t>Keras</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feature Engineering</t>
+  </si>
+  <si>
+    <t>Data Science</t>
   </si>
 </sst>
 </file>
@@ -721,7 +727,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -978,6 +984,9 @@
       <c r="B11" t="s">
         <v>94</v>
       </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
       <c r="H11" t="s">
         <v>67</v>
       </c>
@@ -985,6 +994,9 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
       </c>
       <c r="H12" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Site updated: 2020-07-22 12:43:02
</commit_message>
<xml_diff>
--- a/我博客的标签和categories.xlsx
+++ b/我博客的标签和categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyt\Documents\GitHub Repositories\superlova.github.io\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CDBB76-7884-4064-A281-79A19471F979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2E93D4-0D74-4D0B-8D9A-E9C1DACAE605}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" activeTab="1" xr2:uid="{4D0B95DE-E132-444A-A219-CC0F3237F2C5}"/>
   </bookViews>
   <sheets>
     <sheet name="标签" sheetId="1" r:id="rId1"/>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF1DB48-2DFC-4ED4-8546-E0DC9CD3BD21}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63CC3E8-6D10-4C50-B1BE-58445F00363C}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>